<commit_message>
Do not run sensitivity calculation examples Use hash in readParametersFromXLS Add data importer configuration
</commit_message>
<xml_diff>
--- a/tests/data/Parameters.xlsx
+++ b/tests/data/Parameters.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E74D56-B31E-4B2F-A372-098D65A634C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB3AE2A-2B66-477E-9C9D-761F12C12E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="965" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="3375" windowWidth="28830" windowHeight="15255" tabRatio="965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidSheet" sheetId="12" r:id="rId1"/>
-    <sheet name="ValidSheed_extraColumns" sheetId="34" r:id="rId2"/>
-    <sheet name="InvalidSheet" sheetId="38" r:id="rId3"/>
+    <sheet name="SecondSheet" sheetId="39" r:id="rId2"/>
+    <sheet name="ValidSheed_extraColumns" sheetId="34" r:id="rId3"/>
+    <sheet name="InvalidSheet" sheetId="38" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ValidSheed_extraColumns!$A$1:$D$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ValidSheed_extraColumns!$A$1:$D$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="45">
   <si>
     <t>Container Path</t>
   </si>
@@ -159,6 +160,21 @@
   </si>
   <si>
     <t>Applications|iv infusion GIP</t>
+  </si>
+  <si>
+    <t>Path1</t>
+  </si>
+  <si>
+    <t>Param1</t>
+  </si>
+  <si>
+    <t>Path2</t>
+  </si>
+  <si>
+    <t>DistincParam</t>
+  </si>
+  <si>
+    <t>µmol</t>
   </si>
 </sst>
 </file>
@@ -476,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBAA2E0-75D2-40B2-8FF0-336DC013701A}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C56" sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,27 +523,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -535,13 +548,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -549,10 +562,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -560,27 +573,27 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>5.8240000000000011E-3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -588,13 +601,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>101</v>
+        <v>5.8240000000000011E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -602,10 +615,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -613,16 +626,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>3.3280000000000002E-3</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -630,13 +643,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>106</v>
+        <v>3.3280000000000002E-3</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -644,10 +657,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -655,16 +668,16 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>2.6000000000000003E-3</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -672,13 +685,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>111</v>
+        <v>2.6000000000000003E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -686,10 +699,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -697,16 +710,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>1768</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,13 +727,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>116</v>
+        <v>1768</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -728,10 +741,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -739,16 +752,16 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>585</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -756,13 +769,13 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>121</v>
+        <v>585</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -770,10 +783,10 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -781,16 +794,16 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -798,13 +811,13 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>126</v>
+        <v>273</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -812,10 +825,10 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -823,16 +836,16 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>507</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -840,13 +853,13 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>131</v>
+        <v>507</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -854,10 +867,10 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -865,16 +878,16 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C28">
-        <v>507</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -882,13 +895,13 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>136</v>
+        <v>507</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -896,10 +909,10 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -907,16 +920,16 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>390</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -924,13 +937,13 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>141</v>
+        <v>390</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -938,10 +951,10 @@
         <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -949,16 +962,16 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C34">
-        <v>587.95992099</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -966,13 +979,13 @@
         <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C35">
-        <v>146</v>
+        <v>587.95992099</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -980,10 +993,10 @@
         <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -991,16 +1004,16 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>523.8698478</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1008,13 +1021,13 @@
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>151</v>
+        <v>523.8698478</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1022,10 +1035,10 @@
         <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -1033,16 +1046,16 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C40">
-        <v>702</v>
+        <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1050,13 +1063,13 @@
         <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C41">
-        <v>156</v>
+        <v>702</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1064,10 +1077,10 @@
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -1075,16 +1088,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1092,13 +1105,13 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C44">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1106,10 +1119,10 @@
         <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -1117,16 +1130,16 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>624</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1134,13 +1147,13 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>166</v>
+        <v>624</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1148,10 +1161,10 @@
         <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -1159,16 +1172,16 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>858</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1176,13 +1189,13 @@
         <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>171</v>
+        <v>858</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -1190,10 +1203,10 @@
         <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -1201,16 +1214,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C52">
-        <v>669.44652527999995</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1218,13 +1231,13 @@
         <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C53">
-        <v>176</v>
+        <v>669.44652527999995</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1232,10 +1245,10 @@
         <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -1243,16 +1256,16 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>182</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1260,13 +1273,13 @@
         <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C56">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1274,10 +1287,10 @@
         <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>181</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -1285,16 +1298,16 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C58">
-        <v>171.97674111799998</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1302,13 +1315,13 @@
         <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C59">
-        <v>186</v>
+        <v>171.97674111799998</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -1316,10 +1329,10 @@
         <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -1327,16 +1340,16 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>171.6</v>
+        <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1344,13 +1357,13 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C62">
-        <v>191</v>
+        <v>171.6</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1358,10 +1371,10 @@
         <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>191</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -1369,16 +1382,16 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C64">
-        <v>520</v>
+        <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -1386,13 +1399,13 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C65">
-        <v>196</v>
+        <v>520</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -1400,10 +1413,10 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>196</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -1411,16 +1424,16 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>364</v>
+        <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -1428,13 +1441,13 @@
         <v>33</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C68">
-        <v>201</v>
+        <v>364</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -1442,10 +1455,10 @@
         <v>33</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -1453,16 +1466,16 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>390</v>
+        <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -1470,13 +1483,13 @@
         <v>34</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>206</v>
+        <v>390</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -1484,10 +1497,10 @@
         <v>34</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>206</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -1495,16 +1508,16 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>338</v>
+        <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -1512,13 +1525,13 @@
         <v>35</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>211</v>
+        <v>338</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -1526,10 +1539,10 @@
         <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
@@ -1537,16 +1550,16 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C76">
-        <v>338</v>
+        <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -1554,13 +1567,13 @@
         <v>36</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C77">
-        <v>216</v>
+        <v>338</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -1568,10 +1581,10 @@
         <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -1579,16 +1592,16 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C79">
-        <v>145.6</v>
+        <v>5</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -1596,13 +1609,13 @@
         <v>37</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C80">
-        <v>221</v>
+        <v>145.6</v>
       </c>
       <c r="D80" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -1610,10 +1623,10 @@
         <v>37</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>221</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -1621,12 +1634,26 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>39</v>
       </c>
-      <c r="B82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82">
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83">
         <v>0</v>
       </c>
     </row>
@@ -1636,6 +1663,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642FDAA4-8199-45D2-8CA7-59E49F9483D2}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2FBFB-6EA9-4207-B2AB-7AE2A5B71622}">
   <dimension ref="A1:K82"/>
   <sheetViews>
@@ -2981,11 +3081,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83173C5D-4B2E-49FF-93CF-AD4625E8CB0C}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
@@ -3905,21 +4005,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -4136,24 +4221,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37469586-C926-4B92-80BC-B6950CC29865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4170,4 +4253,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Read params from xls hash (#198)
* Fix col_names argument in steadystate

* Do not run sensitivity calculation examples
Use hash in readParametersFromXLS
Add data importer configuration

* Fixes #37
Add function extendParameterStructure
refactor readParametersFromXLS

* Use named vector instead of hash for extending parameter structure

Co-authored-by: Indrajeet Patil <patilindrajeet.science@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/data/Parameters.xlsx
+++ b/tests/data/Parameters.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E74D56-B31E-4B2F-A372-098D65A634C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB3AE2A-2B66-477E-9C9D-761F12C12E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="965" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57495" yWindow="3375" windowWidth="28830" windowHeight="15255" tabRatio="965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidSheet" sheetId="12" r:id="rId1"/>
-    <sheet name="ValidSheed_extraColumns" sheetId="34" r:id="rId2"/>
-    <sheet name="InvalidSheet" sheetId="38" r:id="rId3"/>
+    <sheet name="SecondSheet" sheetId="39" r:id="rId2"/>
+    <sheet name="ValidSheed_extraColumns" sheetId="34" r:id="rId3"/>
+    <sheet name="InvalidSheet" sheetId="38" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ValidSheed_extraColumns!$A$1:$D$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ValidSheed_extraColumns!$A$1:$D$82</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="45">
   <si>
     <t>Container Path</t>
   </si>
@@ -159,6 +160,21 @@
   </si>
   <si>
     <t>Applications|iv infusion GIP</t>
+  </si>
+  <si>
+    <t>Path1</t>
+  </si>
+  <si>
+    <t>Param1</t>
+  </si>
+  <si>
+    <t>Path2</t>
+  </si>
+  <si>
+    <t>DistincParam</t>
+  </si>
+  <si>
+    <t>µmol</t>
   </si>
 </sst>
 </file>
@@ -476,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBAA2E0-75D2-40B2-8FF0-336DC013701A}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C56" sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,27 +523,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -535,13 +548,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -549,10 +562,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -560,27 +573,27 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>5.8240000000000011E-3</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -588,13 +601,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>101</v>
+        <v>5.8240000000000011E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -602,10 +615,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -613,16 +626,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C10">
-        <v>3.3280000000000002E-3</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -630,13 +643,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>106</v>
+        <v>3.3280000000000002E-3</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -644,10 +657,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -655,16 +668,16 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>2.6000000000000003E-3</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -672,13 +685,13 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C14">
-        <v>111</v>
+        <v>2.6000000000000003E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -686,10 +699,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -697,16 +710,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>1768</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -714,13 +727,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>116</v>
+        <v>1768</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -728,10 +741,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>116</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -739,16 +752,16 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>585</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -756,13 +769,13 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>121</v>
+        <v>585</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -770,10 +783,10 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -781,16 +794,16 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>273</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -798,13 +811,13 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>126</v>
+        <v>273</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -812,10 +825,10 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -823,16 +836,16 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C25">
-        <v>507</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -840,13 +853,13 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>131</v>
+        <v>507</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -854,10 +867,10 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>131</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -865,16 +878,16 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C28">
-        <v>507</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -882,13 +895,13 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C29">
-        <v>136</v>
+        <v>507</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -896,10 +909,10 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>136</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -907,16 +920,16 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C31">
-        <v>390</v>
+        <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -924,13 +937,13 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C32">
-        <v>141</v>
+        <v>390</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -938,10 +951,10 @@
         <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>141</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -949,16 +962,16 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C34">
-        <v>587.95992099</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -966,13 +979,13 @@
         <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C35">
-        <v>146</v>
+        <v>587.95992099</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -980,10 +993,10 @@
         <v>22</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -991,16 +1004,16 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C37">
-        <v>523.8698478</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1008,13 +1021,13 @@
         <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C38">
-        <v>151</v>
+        <v>523.8698478</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1022,10 +1035,10 @@
         <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
         <v>7</v>
@@ -1033,16 +1046,16 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C40">
-        <v>702</v>
+        <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1050,13 +1063,13 @@
         <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C41">
-        <v>156</v>
+        <v>702</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1064,10 +1077,10 @@
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
@@ -1075,16 +1088,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>195</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1092,13 +1105,13 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C44">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1106,10 +1119,10 @@
         <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>161</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
@@ -1117,16 +1130,16 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>624</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1134,13 +1147,13 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>166</v>
+        <v>624</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1148,10 +1161,10 @@
         <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>166</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -1159,16 +1172,16 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C49">
-        <v>858</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1176,13 +1189,13 @@
         <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>171</v>
+        <v>858</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -1190,10 +1203,10 @@
         <v>27</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C51">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
@@ -1201,16 +1214,16 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C52">
-        <v>669.44652527999995</v>
+        <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1218,13 +1231,13 @@
         <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C53">
-        <v>176</v>
+        <v>669.44652527999995</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1232,10 +1245,10 @@
         <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C54">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="D54" t="s">
         <v>7</v>
@@ -1243,16 +1256,16 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>182</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1260,13 +1273,13 @@
         <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C56">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1274,10 +1287,10 @@
         <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C57">
-        <v>5</v>
+        <v>181</v>
       </c>
       <c r="D57" t="s">
         <v>7</v>
@@ -1285,16 +1298,16 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C58">
-        <v>171.97674111799998</v>
+        <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1302,13 +1315,13 @@
         <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C59">
-        <v>186</v>
+        <v>171.97674111799998</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -1316,10 +1329,10 @@
         <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C60">
-        <v>5</v>
+        <v>186</v>
       </c>
       <c r="D60" t="s">
         <v>7</v>
@@ -1327,16 +1340,16 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>171.6</v>
+        <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1344,13 +1357,13 @@
         <v>31</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C62">
-        <v>191</v>
+        <v>171.6</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1358,10 +1371,10 @@
         <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>191</v>
       </c>
       <c r="D63" t="s">
         <v>7</v>
@@ -1369,16 +1382,16 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C64">
-        <v>520</v>
+        <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -1386,13 +1399,13 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C65">
-        <v>196</v>
+        <v>520</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -1400,10 +1413,10 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>196</v>
       </c>
       <c r="D66" t="s">
         <v>7</v>
@@ -1411,16 +1424,16 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>364</v>
+        <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -1428,13 +1441,13 @@
         <v>33</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C68">
-        <v>201</v>
+        <v>364</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -1442,10 +1455,10 @@
         <v>33</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>5</v>
+        <v>201</v>
       </c>
       <c r="D69" t="s">
         <v>7</v>
@@ -1453,16 +1466,16 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>390</v>
+        <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -1470,13 +1483,13 @@
         <v>34</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>206</v>
+        <v>390</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -1484,10 +1497,10 @@
         <v>34</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>5</v>
+        <v>206</v>
       </c>
       <c r="D72" t="s">
         <v>7</v>
@@ -1495,16 +1508,16 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>338</v>
+        <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -1512,13 +1525,13 @@
         <v>35</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>211</v>
+        <v>338</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -1526,10 +1539,10 @@
         <v>35</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
         <v>7</v>
@@ -1537,16 +1550,16 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C76">
-        <v>338</v>
+        <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -1554,13 +1567,13 @@
         <v>36</v>
       </c>
       <c r="B77" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C77">
-        <v>216</v>
+        <v>338</v>
       </c>
       <c r="D77" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -1568,10 +1581,10 @@
         <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C78">
-        <v>5</v>
+        <v>216</v>
       </c>
       <c r="D78" t="s">
         <v>7</v>
@@ -1579,16 +1592,16 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C79">
-        <v>145.6</v>
+        <v>5</v>
       </c>
       <c r="D79" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -1596,13 +1609,13 @@
         <v>37</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C80">
-        <v>221</v>
+        <v>145.6</v>
       </c>
       <c r="D80" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -1610,10 +1623,10 @@
         <v>37</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C81">
-        <v>5</v>
+        <v>221</v>
       </c>
       <c r="D81" t="s">
         <v>7</v>
@@ -1621,12 +1634,26 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>39</v>
       </c>
-      <c r="B82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82">
+      <c r="B83" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83">
         <v>0</v>
       </c>
     </row>
@@ -1636,6 +1663,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642FDAA4-8199-45D2-8CA7-59E49F9483D2}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34F2FBFB-6EA9-4207-B2AB-7AE2A5B71622}">
   <dimension ref="A1:K82"/>
   <sheetViews>
@@ -2981,11 +3081,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83173C5D-4B2E-49FF-93CF-AD4625E8CB0C}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
@@ -3905,21 +4005,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -4136,24 +4221,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37469586-C926-4B92-80BC-B6950CC29865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4170,4 +4253,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added test for loading empty sheet.
</commit_message>
<xml_diff>
--- a/tests/data/Parameters.xlsx
+++ b/tests/data/Parameters.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB3AE2A-2B66-477E-9C9D-761F12C12E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32660838-E945-410D-9FAC-6379575E4078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57495" yWindow="3375" windowWidth="28830" windowHeight="15255" tabRatio="965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="965" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidSheet" sheetId="12" r:id="rId1"/>
     <sheet name="SecondSheet" sheetId="39" r:id="rId2"/>
     <sheet name="ValidSheed_extraColumns" sheetId="34" r:id="rId3"/>
     <sheet name="InvalidSheet" sheetId="38" r:id="rId4"/>
+    <sheet name="EmptySheet" sheetId="40" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ValidSheed_extraColumns!$A$1:$D$82</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="45">
   <si>
     <t>Container Path</t>
   </si>
@@ -495,7 +496,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1666,7 +1667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642FDAA4-8199-45D2-8CA7-59E49F9483D2}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4004,7 +4005,51 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC4BB1E-E085-43E7-8630-6B66B818F108}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -4221,22 +4266,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37469586-C926-4B92-80BC-B6950CC29865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4253,21 +4300,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added test for loading empty sheet. (#224)
* Added test for loading empty sheet.

* skip unit NA replacement if no data

* Converting the unit column to character type before replacing NAs

* Remove column types argument

Co-authored-by: Indrajeet Patil <patilindrajeet.science@gmail.com>
</commit_message>
<xml_diff>
--- a/tests/data/Parameters.xlsx
+++ b/tests/data/Parameters.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB3AE2A-2B66-477E-9C9D-761F12C12E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32660838-E945-410D-9FAC-6379575E4078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57495" yWindow="3375" windowWidth="28830" windowHeight="15255" tabRatio="965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="965" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidSheet" sheetId="12" r:id="rId1"/>
     <sheet name="SecondSheet" sheetId="39" r:id="rId2"/>
     <sheet name="ValidSheed_extraColumns" sheetId="34" r:id="rId3"/>
     <sheet name="InvalidSheet" sheetId="38" r:id="rId4"/>
+    <sheet name="EmptySheet" sheetId="40" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ValidSheed_extraColumns!$A$1:$D$82</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="45">
   <si>
     <t>Container Path</t>
   </si>
@@ -495,7 +496,7 @@
   <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1666,7 +1667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642FDAA4-8199-45D2-8CA7-59E49F9483D2}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -4004,7 +4005,51 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC4BB1E-E085-43E7-8630-6B66B818F108}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6960b7ce0e258e5d224c1a71edff679">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7db7ba54f101f424e932c64edcbdaa0" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -4221,22 +4266,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37469586-C926-4B92-80BC-B6950CC29865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4253,21 +4300,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253E2BCE-BEE3-46CA-82C7-E211846F5250}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D118C015-E179-46FB-B6E8-2D926D65EB7E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>